<commit_message>
Sorting the output of wines Deleted the extra code
</commit_message>
<xml_diff>
--- a/wine.xlsx
+++ b/wine.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Илья\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lilu/dev/wine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F64F38-63D8-492D-A065-4488BEC8CFAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE1E266-452D-8F4B-A49A-81E02C84B73E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>Название</t>
   </si>
@@ -406,20 +406,19 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" customWidth="1"/>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
     <col min="2" max="2" width="27.6640625" customWidth="1"/>
-    <col min="3" max="3" width="23.44140625" customWidth="1"/>
+    <col min="3" max="3" width="23.5" customWidth="1"/>
     <col min="4" max="4" width="32.33203125" customWidth="1"/>
-    <col min="5" max="5" width="24.5546875" customWidth="1"/>
-    <col min="6" max="6" width="24.44140625" customWidth="1"/>
+    <col min="5" max="6" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -439,7 +438,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
@@ -459,7 +458,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
@@ -475,7 +474,7 @@
       </c>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
@@ -493,7 +492,7 @@
       </c>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
@@ -509,9 +508,11 @@
       <c r="E5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F5" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
@@ -529,7 +530,7 @@
       </c>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -547,7 +548,7 @@
       </c>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>17</v>
       </c>
@@ -565,7 +566,7 @@
       </c>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
         <v>14</v>
       </c>
@@ -583,7 +584,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
         <v>14</v>
       </c>

</xml_diff>